<commit_message>
added requirements.txt and folder for png
</commit_message>
<xml_diff>
--- a/façonneur.xlsx
+++ b/façonneur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" activeTab="7"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Ressources" sheetId="1" r:id="rId1"/>
@@ -2257,7 +2257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H74"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -3208,8 +3208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6980,17 +6980,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="H79:J79"/>
-    <mergeCell ref="M79:O79"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="M46:O46"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="H68:J68"/>
-    <mergeCell ref="M68:O68"/>
     <mergeCell ref="C90:E90"/>
     <mergeCell ref="H90:J90"/>
     <mergeCell ref="M90:O90"/>
@@ -7007,6 +6996,17 @@
     <mergeCell ref="H24:J24"/>
     <mergeCell ref="M24:O24"/>
     <mergeCell ref="C35:E35"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="H79:J79"/>
+    <mergeCell ref="M79:O79"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="M46:O46"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="H68:J68"/>
+    <mergeCell ref="M68:O68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -8808,7 +8808,7 @@
   <dimension ref="B1:K45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9459,8 +9459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9515,46 +9515,46 @@
       </c>
       <c r="C4" s="12">
         <f>Raw!D2</f>
-        <v>11997</v>
+        <v>11372</v>
       </c>
       <c r="E4" s="75" t="s">
         <v>164</v>
       </c>
       <c r="F4" s="71">
         <f>C4</f>
-        <v>11997</v>
+        <v>11372</v>
       </c>
       <c r="G4" s="72">
         <f>F4*3</f>
-        <v>35991</v>
+        <v>34116</v>
       </c>
       <c r="H4" s="72">
         <f>G4*3</f>
-        <v>107973</v>
+        <v>102348</v>
       </c>
       <c r="I4" s="93">
         <f t="shared" ref="I4:I12" si="0">C18</f>
-        <v>38995</v>
+        <v>35454</v>
       </c>
       <c r="J4" s="93">
         <f>C32</f>
-        <v>109996</v>
+        <v>110798</v>
       </c>
       <c r="K4" s="11">
         <f>I4-G4</f>
-        <v>3004</v>
+        <v>1338</v>
       </c>
       <c r="L4" s="94">
         <f t="shared" ref="L4:L14" si="1">1-(G4/I4)</f>
-        <v>7.7035517374022255E-2</v>
+        <v>3.7739042139109835E-2</v>
       </c>
       <c r="M4" s="11">
         <f t="shared" ref="M4:M11" si="2">J4-H4</f>
-        <v>2023</v>
+        <v>8450</v>
       </c>
       <c r="N4" s="69">
         <f>1-(H4/J4)</f>
-        <v>1.8391577875559117E-2</v>
+        <v>7.626491452914308E-2</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
@@ -10096,7 +10096,7 @@
       </c>
       <c r="C18" s="20">
         <f>Raw!D28</f>
-        <v>38995</v>
+        <v>35454</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -10216,7 +10216,7 @@
       </c>
       <c r="C32" s="20">
         <f>Raw!D54</f>
-        <v>109996</v>
+        <v>110798</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -10334,8 +10334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="A1:D68"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="K67" sqref="K67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10347,7 +10347,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D2">
-        <v>11997</v>
+        <v>11372</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -10477,7 +10477,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D28">
-        <v>38995</v>
+        <v>35454</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -10607,7 +10607,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D54">
-        <v>109996</v>
+        <v>110798</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix excel and did 1 pass of runes with success
</commit_message>
<xml_diff>
--- a/façonneur.xlsx
+++ b/façonneur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" activeTab="8"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Ressources" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="241">
   <si>
     <t>Ardonite</t>
   </si>
@@ -644,6 +644,108 @@
   </si>
   <si>
     <t>Rune Do Terre</t>
+  </si>
+  <si>
+    <t>9999</t>
+  </si>
+  <si>
+    <t>9000</t>
+  </si>
+  <si>
+    <t>3681</t>
+  </si>
+  <si>
+    <t>5900</t>
+  </si>
+  <si>
+    <t>14850</t>
+  </si>
+  <si>
+    <t>16997</t>
+  </si>
+  <si>
+    <t>11000</t>
+  </si>
+  <si>
+    <t>28000</t>
+  </si>
+  <si>
+    <t>38983</t>
+  </si>
+  <si>
+    <t>99995</t>
+  </si>
+  <si>
+    <t>120990</t>
+  </si>
+  <si>
+    <t>111759</t>
+  </si>
+  <si>
+    <t>76608</t>
+  </si>
+  <si>
+    <t>35454</t>
+  </si>
+  <si>
+    <t>27989</t>
+  </si>
+  <si>
+    <t>12489</t>
+  </si>
+  <si>
+    <t>25436</t>
+  </si>
+  <si>
+    <t>58999</t>
+  </si>
+  <si>
+    <t>53925</t>
+  </si>
+  <si>
+    <t>38785</t>
+  </si>
+  <si>
+    <t>92089</t>
+  </si>
+  <si>
+    <t>129899</t>
+  </si>
+  <si>
+    <t>336813</t>
+  </si>
+  <si>
+    <t>419973</t>
+  </si>
+  <si>
+    <t>238993</t>
+  </si>
+  <si>
+    <t>228999</t>
+  </si>
+  <si>
+    <t>110798</t>
+  </si>
+  <si>
+    <t>94645</t>
+  </si>
+  <si>
+    <t>37354</t>
+  </si>
+  <si>
+    <t>77982</t>
+  </si>
+  <si>
+    <t>148680</t>
+  </si>
+  <si>
+    <t>169159</t>
+  </si>
+  <si>
+    <t>98967</t>
+  </si>
+  <si>
+    <t>200000</t>
   </si>
 </sst>
 </file>
@@ -6980,6 +7082,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="H79:J79"/>
+    <mergeCell ref="M79:O79"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="M46:O46"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="H68:J68"/>
+    <mergeCell ref="M68:O68"/>
     <mergeCell ref="C90:E90"/>
     <mergeCell ref="H90:J90"/>
     <mergeCell ref="M90:O90"/>
@@ -6996,17 +7109,6 @@
     <mergeCell ref="H24:J24"/>
     <mergeCell ref="M24:O24"/>
     <mergeCell ref="C35:E35"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="H79:J79"/>
-    <mergeCell ref="M79:O79"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="M46:O46"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="H68:J68"/>
-    <mergeCell ref="M68:O68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -9459,8 +9561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9513,336 +9615,336 @@
       <c r="B4" s="95" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="12" t="str">
         <f>Raw!D2</f>
-        <v>11372</v>
+        <v>9999</v>
       </c>
       <c r="E4" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="F4" s="71">
+      <c r="F4" s="71" t="str">
         <f>C4</f>
-        <v>11372</v>
+        <v>9999</v>
       </c>
       <c r="G4" s="72">
         <f>F4*3</f>
-        <v>34116</v>
+        <v>29997</v>
       </c>
       <c r="H4" s="72">
         <f>G4*3</f>
-        <v>102348</v>
-      </c>
-      <c r="I4" s="93">
+        <v>89991</v>
+      </c>
+      <c r="I4" s="93" t="str">
         <f t="shared" ref="I4:I12" si="0">C18</f>
         <v>35454</v>
       </c>
-      <c r="J4" s="93">
+      <c r="J4" s="93" t="str">
         <f>C32</f>
         <v>110798</v>
       </c>
       <c r="K4" s="11">
         <f>I4-G4</f>
-        <v>1338</v>
+        <v>5457</v>
       </c>
       <c r="L4" s="94">
         <f t="shared" ref="L4:L14" si="1">1-(G4/I4)</f>
-        <v>3.7739042139109835E-2</v>
+        <v>0.15391775258080898</v>
       </c>
       <c r="M4" s="11">
         <f t="shared" ref="M4:M11" si="2">J4-H4</f>
-        <v>8450</v>
+        <v>20807</v>
       </c>
       <c r="N4" s="69">
         <f>1-(H4/J4)</f>
-        <v>7.626491452914308E-2</v>
+        <v>0.18779219841513384</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="96" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="3" t="str">
         <f>Raw!D4</f>
-        <v>6100</v>
+        <v>9000</v>
       </c>
       <c r="E5" s="76" t="s">
         <v>165</v>
       </c>
-      <c r="F5" s="73">
+      <c r="F5" s="73" t="str">
         <f>C5</f>
-        <v>6100</v>
+        <v>9000</v>
       </c>
       <c r="G5" s="74">
         <f t="shared" ref="G5:H16" si="3">F5*3</f>
-        <v>18300</v>
+        <v>27000</v>
       </c>
       <c r="H5" s="74">
         <f t="shared" si="3"/>
-        <v>54900</v>
-      </c>
-      <c r="I5" s="91">
+        <v>81000</v>
+      </c>
+      <c r="I5" s="91" t="str">
         <f t="shared" si="0"/>
-        <v>23317</v>
-      </c>
-      <c r="J5" s="91">
+        <v>27989</v>
+      </c>
+      <c r="J5" s="91" t="str">
         <f t="shared" ref="J5:J11" si="4">C33</f>
-        <v>56999</v>
+        <v>94645</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" ref="K5:K16" si="5">I5-G5</f>
-        <v>5017</v>
+        <v>989</v>
       </c>
       <c r="L5" s="92">
         <f t="shared" si="1"/>
-        <v>0.21516490114508724</v>
+        <v>3.5335310300475209E-2</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" si="2"/>
-        <v>2099</v>
+        <v>13645</v>
       </c>
       <c r="N5" s="70">
         <f t="shared" ref="N5:N11" si="6">1-(H5/J5)</f>
-        <v>3.6825207459780018E-2</v>
+        <v>0.14417032067198476</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="96" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="3" t="str">
         <f>Raw!D6</f>
-        <v>14749</v>
+        <v>3681</v>
       </c>
       <c r="E6" s="76" t="s">
         <v>166</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="73" t="str">
         <f t="shared" ref="F6:F16" si="7">C6</f>
-        <v>14749</v>
+        <v>3681</v>
       </c>
       <c r="G6" s="74">
         <f t="shared" si="3"/>
-        <v>44247</v>
+        <v>11043</v>
       </c>
       <c r="H6" s="74">
         <f t="shared" si="3"/>
-        <v>132741</v>
-      </c>
-      <c r="I6" s="91">
+        <v>33129</v>
+      </c>
+      <c r="I6" s="91" t="str">
         <f t="shared" si="0"/>
-        <v>61897</v>
-      </c>
-      <c r="J6" s="91">
+        <v>12489</v>
+      </c>
+      <c r="J6" s="91" t="str">
         <f t="shared" si="4"/>
-        <v>70887</v>
+        <v>37354</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" si="5"/>
-        <v>17650</v>
+        <v>1446</v>
       </c>
       <c r="L6" s="92">
         <f t="shared" si="1"/>
-        <v>0.28515113818117199</v>
+        <v>0.11578188806149414</v>
       </c>
       <c r="M6" s="2">
         <f t="shared" si="2"/>
-        <v>-61854</v>
+        <v>4225</v>
       </c>
       <c r="N6" s="70">
         <f t="shared" si="6"/>
-        <v>-0.87257183968851826</v>
+        <v>0.11310703003694389</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="96" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="3" t="str">
         <f>Raw!D8</f>
-        <v>7478</v>
+        <v>5900</v>
       </c>
       <c r="E7" s="76" t="s">
         <v>167</v>
       </c>
-      <c r="F7" s="73">
+      <c r="F7" s="73" t="str">
         <f t="shared" si="7"/>
-        <v>7478</v>
+        <v>5900</v>
       </c>
       <c r="G7" s="74">
         <f t="shared" si="3"/>
-        <v>22434</v>
+        <v>17700</v>
       </c>
       <c r="H7" s="74">
         <f t="shared" si="3"/>
-        <v>67302</v>
-      </c>
-      <c r="I7" s="91">
+        <v>53100</v>
+      </c>
+      <c r="I7" s="91" t="str">
         <f t="shared" si="0"/>
-        <v>32528</v>
-      </c>
-      <c r="J7" s="91">
+        <v>25436</v>
+      </c>
+      <c r="J7" s="91" t="str">
         <f t="shared" si="4"/>
-        <v>78776</v>
+        <v>77982</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" si="5"/>
-        <v>10094</v>
+        <v>7736</v>
       </c>
       <c r="L7" s="92">
         <f t="shared" si="1"/>
-        <v>0.31031726512543045</v>
+        <v>0.30413587041987733</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" si="2"/>
-        <v>11474</v>
+        <v>24882</v>
       </c>
       <c r="N7" s="70">
         <f t="shared" si="6"/>
-        <v>0.14565349852747034</v>
+        <v>0.31907363237670228</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="96" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="3" t="str">
         <f>Raw!D10</f>
-        <v>6900</v>
+        <v>14850</v>
       </c>
       <c r="E8" s="76" t="s">
         <v>168</v>
       </c>
-      <c r="F8" s="73">
+      <c r="F8" s="73" t="str">
         <f t="shared" si="7"/>
-        <v>6900</v>
+        <v>14850</v>
       </c>
       <c r="G8" s="74">
         <f t="shared" si="3"/>
-        <v>20700</v>
+        <v>44550</v>
       </c>
       <c r="H8" s="74">
         <f t="shared" si="3"/>
-        <v>62100</v>
-      </c>
-      <c r="I8" s="91">
+        <v>133650</v>
+      </c>
+      <c r="I8" s="91" t="str">
         <f t="shared" si="0"/>
-        <v>33898</v>
-      </c>
-      <c r="J8" s="91">
+        <v>58999</v>
+      </c>
+      <c r="J8" s="91" t="str">
         <f t="shared" si="4"/>
-        <v>100000</v>
+        <v>148680</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="5"/>
-        <v>13198</v>
+        <v>14449</v>
       </c>
       <c r="L8" s="92">
         <f t="shared" si="1"/>
-        <v>0.38934450410053689</v>
+        <v>0.24490245597383009</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" si="2"/>
-        <v>37900</v>
+        <v>15030</v>
       </c>
       <c r="N8" s="70">
         <f t="shared" si="6"/>
-        <v>0.379</v>
+        <v>0.10108958837772397</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="96" t="s">
         <v>137</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="3" t="str">
         <f>Raw!D12</f>
-        <v>19998</v>
+        <v>16997</v>
       </c>
       <c r="E9" s="76" t="s">
         <v>169</v>
       </c>
-      <c r="F9" s="73">
+      <c r="F9" s="73" t="str">
         <f t="shared" si="7"/>
-        <v>19998</v>
+        <v>16997</v>
       </c>
       <c r="G9" s="74">
         <f t="shared" si="3"/>
-        <v>59994</v>
+        <v>50991</v>
       </c>
       <c r="H9" s="74">
         <f t="shared" si="3"/>
-        <v>179982</v>
-      </c>
-      <c r="I9" s="91">
+        <v>152973</v>
+      </c>
+      <c r="I9" s="91" t="str">
         <f t="shared" si="0"/>
-        <v>72149</v>
-      </c>
-      <c r="J9" s="91">
+        <v>53925</v>
+      </c>
+      <c r="J9" s="91" t="str">
         <f t="shared" si="4"/>
-        <v>180000</v>
+        <v>169159</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="5"/>
-        <v>12155</v>
+        <v>2934</v>
       </c>
       <c r="L9" s="92">
         <f t="shared" si="1"/>
-        <v>0.16847080347613963</v>
+        <v>5.4408901251738473E-2</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>16186</v>
       </c>
       <c r="N9" s="70">
         <f t="shared" si="6"/>
-        <v>9.9999999999988987E-5</v>
+        <v>9.5685124646043063E-2</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="96" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="3" t="str">
         <f>Raw!D14</f>
-        <v>10997</v>
+        <v>11000</v>
       </c>
       <c r="E10" s="76" t="s">
         <v>170</v>
       </c>
-      <c r="F10" s="73">
+      <c r="F10" s="73" t="str">
         <f t="shared" si="7"/>
-        <v>10997</v>
+        <v>11000</v>
       </c>
       <c r="G10" s="74">
         <f t="shared" si="3"/>
-        <v>32991</v>
+        <v>33000</v>
       </c>
       <c r="H10" s="74">
         <f t="shared" si="3"/>
-        <v>98973</v>
-      </c>
-      <c r="I10" s="91">
+        <v>99000</v>
+      </c>
+      <c r="I10" s="91" t="str">
         <f t="shared" si="0"/>
-        <v>50492</v>
-      </c>
-      <c r="J10" s="91">
+        <v>38785</v>
+      </c>
+      <c r="J10" s="91" t="str">
         <f t="shared" si="4"/>
-        <v>96998</v>
+        <v>98967</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" si="5"/>
-        <v>17501</v>
+        <v>5785</v>
       </c>
       <c r="L10" s="92">
         <f t="shared" si="1"/>
-        <v>0.34660936385962138</v>
+        <v>0.14915560139229078</v>
       </c>
       <c r="M10" s="2">
         <f t="shared" si="2"/>
-        <v>-1975</v>
+        <v>-33</v>
       </c>
       <c r="N10" s="70">
         <f t="shared" si="6"/>
-        <v>-2.0361244561743597E-2</v>
+        <v>-3.3344448149374983E-4</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
@@ -9867,9 +9969,9 @@
         <f t="shared" si="3"/>
         <v>494901</v>
       </c>
-      <c r="I11" s="91">
+      <c r="I11" s="91" t="str">
         <f t="shared" si="0"/>
-        <v>169996</v>
+        <v>92089</v>
       </c>
       <c r="J11" s="91">
         <f t="shared" si="4"/>
@@ -9877,11 +9979,11 @@
       </c>
       <c r="K11" s="2">
         <f t="shared" si="5"/>
-        <v>5029</v>
+        <v>-72878</v>
       </c>
       <c r="L11" s="92">
         <f t="shared" si="1"/>
-        <v>2.9583049012917972E-2</v>
+        <v>-0.79138659340420681</v>
       </c>
       <c r="M11" s="2">
         <f t="shared" si="2"/>
@@ -9896,37 +9998,37 @@
       <c r="B12" s="96" t="s">
         <v>202</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="3" t="str">
         <f>Raw!D18</f>
-        <v>124992</v>
+        <v>38983</v>
       </c>
       <c r="E12" s="76" t="s">
         <v>200</v>
       </c>
-      <c r="F12" s="73">
+      <c r="F12" s="73" t="str">
         <f>C12</f>
-        <v>124992</v>
+        <v>38983</v>
       </c>
       <c r="G12" s="74">
         <f t="shared" si="3"/>
-        <v>374976</v>
+        <v>116949</v>
       </c>
       <c r="H12" s="74">
         <f t="shared" si="3"/>
-        <v>1124928</v>
-      </c>
-      <c r="I12" s="91">
+        <v>350847</v>
+      </c>
+      <c r="I12" s="91" t="str">
         <f t="shared" si="0"/>
-        <v>319990</v>
+        <v>129899</v>
       </c>
       <c r="J12" s="91"/>
       <c r="K12" s="2">
         <f t="shared" si="5"/>
-        <v>-54986</v>
+        <v>12950</v>
       </c>
       <c r="L12" s="92">
         <f t="shared" si="1"/>
-        <v>-0.17183661989437171</v>
+        <v>9.9692838282049889E-2</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="70"/>
@@ -9935,37 +10037,37 @@
       <c r="B13" s="96" t="s">
         <v>140</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="3" t="str">
         <f>Raw!D20</f>
-        <v>117996</v>
+        <v>99995</v>
       </c>
       <c r="E13" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="F13" s="73">
+      <c r="F13" s="73" t="str">
         <f t="shared" si="7"/>
-        <v>117996</v>
+        <v>99995</v>
       </c>
       <c r="G13" s="74">
         <f t="shared" si="3"/>
-        <v>353988</v>
+        <v>299985</v>
       </c>
       <c r="H13" s="74">
         <f t="shared" si="3"/>
-        <v>1061964</v>
-      </c>
-      <c r="I13" s="91">
+        <v>899955</v>
+      </c>
+      <c r="I13" s="91" t="str">
         <f t="shared" ref="I13:I16" si="8">C27</f>
-        <v>240000</v>
+        <v>336813</v>
       </c>
       <c r="J13" s="91"/>
       <c r="K13" s="2">
         <f t="shared" si="5"/>
-        <v>-113988</v>
+        <v>36828</v>
       </c>
       <c r="L13" s="92">
         <f t="shared" si="1"/>
-        <v>-0.47494999999999998</v>
+        <v>0.10934257288168803</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="3"/>
@@ -9974,37 +10076,37 @@
       <c r="B14" s="96" t="s">
         <v>141</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="3" t="str">
         <f>Raw!D22</f>
-        <v>107772</v>
+        <v>120990</v>
       </c>
       <c r="E14" s="76" t="s">
         <v>173</v>
       </c>
-      <c r="F14" s="73">
+      <c r="F14" s="73" t="str">
         <f t="shared" si="7"/>
-        <v>107772</v>
+        <v>120990</v>
       </c>
       <c r="G14" s="74">
         <f t="shared" si="3"/>
-        <v>323316</v>
+        <v>362970</v>
       </c>
       <c r="H14" s="74">
         <f t="shared" si="3"/>
-        <v>969948</v>
-      </c>
-      <c r="I14" s="91">
+        <v>1088910</v>
+      </c>
+      <c r="I14" s="91" t="str">
         <f t="shared" si="8"/>
-        <v>289994</v>
+        <v>419973</v>
       </c>
       <c r="J14" s="91"/>
       <c r="K14" s="2">
         <f t="shared" si="5"/>
-        <v>-33322</v>
+        <v>57003</v>
       </c>
       <c r="L14" s="92">
         <f t="shared" si="1"/>
-        <v>-0.11490582563777174</v>
+        <v>0.13573015408133382</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="3"/>
@@ -10013,37 +10115,37 @@
       <c r="B15" s="96" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="3" t="str">
         <f>Raw!D24</f>
-        <v>57190</v>
+        <v>111759</v>
       </c>
       <c r="E15" s="76" t="s">
         <v>174</v>
       </c>
-      <c r="F15" s="73">
+      <c r="F15" s="73" t="str">
         <f t="shared" si="7"/>
-        <v>57190</v>
+        <v>111759</v>
       </c>
       <c r="G15" s="74">
         <f t="shared" si="3"/>
-        <v>171570</v>
+        <v>335277</v>
       </c>
       <c r="H15" s="74">
         <f t="shared" si="3"/>
-        <v>514710</v>
-      </c>
-      <c r="I15" s="91">
+        <v>1005831</v>
+      </c>
+      <c r="I15" s="91" t="str">
         <f t="shared" si="8"/>
-        <v>299995</v>
+        <v>238993</v>
       </c>
       <c r="J15" s="91"/>
       <c r="K15" s="2">
         <f t="shared" si="5"/>
-        <v>128425</v>
+        <v>-96284</v>
       </c>
       <c r="L15" s="92">
         <f>1-(G15/I15)</f>
-        <v>0.42809046817446961</v>
+        <v>-0.40287372433502244</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="3"/>
@@ -10052,37 +10154,37 @@
       <c r="B16" s="97" t="s">
         <v>143</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="4" t="str">
         <f>Raw!D26</f>
-        <v>118394</v>
+        <v>76608</v>
       </c>
       <c r="E16" s="76" t="s">
         <v>175</v>
       </c>
-      <c r="F16" s="73">
+      <c r="F16" s="73" t="str">
         <f t="shared" si="7"/>
-        <v>118394</v>
+        <v>76608</v>
       </c>
       <c r="G16" s="74">
         <f t="shared" si="3"/>
-        <v>355182</v>
+        <v>229824</v>
       </c>
       <c r="H16" s="74">
         <f t="shared" si="3"/>
-        <v>1065546</v>
-      </c>
-      <c r="I16" s="91">
+        <v>689472</v>
+      </c>
+      <c r="I16" s="91" t="str">
         <f t="shared" si="8"/>
-        <v>329994</v>
+        <v>228999</v>
       </c>
       <c r="J16" s="91"/>
       <c r="K16" s="2">
         <f t="shared" si="5"/>
-        <v>-25188</v>
+        <v>-825</v>
       </c>
       <c r="L16" s="92">
         <f>1-(G16/I16)</f>
-        <v>-7.6328660521100433E-2</v>
+        <v>-3.60263581937037E-3</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="3"/>
@@ -10094,7 +10196,7 @@
       <c r="B18" s="75" t="s">
         <v>144</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="20" t="str">
         <f>Raw!D28</f>
         <v>35454</v>
       </c>
@@ -10103,108 +10205,108 @@
       <c r="B19" s="76" t="s">
         <v>145</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="21" t="str">
         <f>Raw!D30</f>
-        <v>23317</v>
+        <v>27989</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="76" t="s">
         <v>146</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="21" t="str">
         <f>Raw!D32</f>
-        <v>61897</v>
+        <v>12489</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="76" t="s">
         <v>147</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="21" t="str">
         <f>Raw!D34</f>
-        <v>32528</v>
+        <v>25436</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="76" t="s">
         <v>148</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="21" t="str">
         <f>Raw!D36</f>
-        <v>33898</v>
+        <v>58999</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="76" t="s">
         <v>149</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="21" t="str">
         <f>Raw!D38</f>
-        <v>72149</v>
+        <v>53925</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="76" t="s">
         <v>150</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="21" t="str">
         <f>Raw!D40</f>
-        <v>50492</v>
+        <v>38785</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="76" t="s">
         <v>151</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="21" t="str">
         <f>Raw!D42</f>
-        <v>169996</v>
+        <v>92089</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="76" t="s">
         <v>199</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="21" t="str">
         <f>Raw!D44</f>
-        <v>319990</v>
+        <v>129899</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="76" t="s">
         <v>152</v>
       </c>
-      <c r="C27" s="21">
+      <c r="C27" s="21" t="str">
         <f>Raw!D46</f>
-        <v>240000</v>
+        <v>336813</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="76" t="s">
         <v>153</v>
       </c>
-      <c r="C28" s="21">
+      <c r="C28" s="21" t="str">
         <f>Raw!D48</f>
-        <v>289994</v>
+        <v>419973</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="76" t="s">
         <v>154</v>
       </c>
-      <c r="C29" s="21">
+      <c r="C29" s="21" t="str">
         <f>Raw!D50</f>
-        <v>299995</v>
+        <v>238993</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="77" t="s">
         <v>155</v>
       </c>
-      <c r="C30" s="22">
+      <c r="C30" s="22" t="str">
         <f>Raw!D52</f>
-        <v>329994</v>
+        <v>228999</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10214,7 +10316,7 @@
       <c r="B32" s="75" t="s">
         <v>156</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C32" s="20" t="str">
         <f>Raw!D54</f>
         <v>110798</v>
       </c>
@@ -10223,54 +10325,54 @@
       <c r="B33" s="76" t="s">
         <v>157</v>
       </c>
-      <c r="C33" s="21">
+      <c r="C33" s="21" t="str">
         <f>Raw!D56</f>
-        <v>56999</v>
+        <v>94645</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="76" t="s">
         <v>158</v>
       </c>
-      <c r="C34" s="21">
+      <c r="C34" s="21" t="str">
         <f>Raw!D58</f>
-        <v>70887</v>
+        <v>37354</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="76" t="s">
         <v>159</v>
       </c>
-      <c r="C35" s="21">
+      <c r="C35" s="21" t="str">
         <f>Raw!D60</f>
-        <v>78776</v>
+        <v>77982</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="76" t="s">
         <v>160</v>
       </c>
-      <c r="C36" s="21">
+      <c r="C36" s="21" t="str">
         <f>Raw!D62</f>
-        <v>100000</v>
+        <v>148680</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="76" t="s">
         <v>161</v>
       </c>
-      <c r="C37" s="21">
+      <c r="C37" s="21" t="str">
         <f>Raw!D64</f>
-        <v>180000</v>
+        <v>169159</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="76" t="s">
         <v>162</v>
       </c>
-      <c r="C38" s="21">
+      <c r="C38" s="21" t="str">
         <f>Raw!D66</f>
-        <v>96998</v>
+        <v>98967</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10334,11 +10436,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="K67" sqref="K67"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -10346,8 +10451,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D2">
-        <v>11372</v>
+      <c r="D2" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -10356,8 +10461,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D4">
-        <v>6100</v>
+      <c r="D4" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -10366,8 +10471,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6">
-        <v>14749</v>
+      <c r="D6" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -10376,8 +10481,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D8">
-        <v>7478</v>
+      <c r="D8" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -10386,8 +10491,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D10">
-        <v>6900</v>
+      <c r="D10" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -10396,8 +10501,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D12">
-        <v>19998</v>
+      <c r="D12" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -10406,8 +10511,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D14">
-        <v>10997</v>
+      <c r="D14" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -10416,8 +10521,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D16">
-        <v>54985</v>
+      <c r="D16" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -10426,8 +10531,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D18">
-        <v>124992</v>
+      <c r="D18" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -10436,8 +10541,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D20">
-        <v>117996</v>
+      <c r="D20" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -10446,8 +10551,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D22">
-        <v>107772</v>
+      <c r="D22" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -10456,8 +10561,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D24">
-        <v>57190</v>
+      <c r="D24" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -10466,8 +10571,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D26">
-        <v>118394</v>
+      <c r="D26" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -10476,8 +10581,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D28">
-        <v>35454</v>
+      <c r="D28" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -10486,8 +10591,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D30">
-        <v>23317</v>
+      <c r="D30" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -10496,8 +10601,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D32">
-        <v>61897</v>
+      <c r="D32" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -10506,8 +10611,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D34">
-        <v>32528</v>
+      <c r="D34" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -10516,8 +10621,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D36">
-        <v>33898</v>
+      <c r="D36" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -10526,8 +10631,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D38">
-        <v>72149</v>
+      <c r="D38" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -10536,8 +10641,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D40">
-        <v>50492</v>
+      <c r="D40" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -10546,8 +10651,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D42">
-        <v>169996</v>
+      <c r="D42" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -10556,8 +10661,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D44">
-        <v>319990</v>
+      <c r="D44" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -10566,8 +10671,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D46">
-        <v>240000</v>
+      <c r="D46" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -10576,8 +10681,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D48">
-        <v>289994</v>
+      <c r="D48" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -10586,8 +10691,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D50">
-        <v>299995</v>
+      <c r="D50" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -10596,8 +10701,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D52">
-        <v>329994</v>
+      <c r="D52" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -10606,8 +10711,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D54">
-        <v>110798</v>
+      <c r="D54" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -10616,8 +10721,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D56">
-        <v>56999</v>
+      <c r="D56" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -10626,8 +10731,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D58">
-        <v>70887</v>
+      <c r="D58" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -10636,8 +10741,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D60">
-        <v>78776</v>
+      <c r="D60" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -10646,8 +10751,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D62">
-        <v>100000</v>
+      <c r="D62" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -10656,8 +10761,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D64">
-        <v>180000</v>
+      <c r="D64" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -10666,8 +10771,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D66">
-        <v>96998</v>
+      <c r="D66" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -10676,8 +10781,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D68">
-        <v>529988</v>
+      <c r="D68" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix runes pui in sheet
</commit_message>
<xml_diff>
--- a/façonneur.xlsx
+++ b/façonneur.xlsx
@@ -1780,22 +1780,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1814,71 +1798,27 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1963,6 +1903,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3422,7 +3382,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3710,29 +3670,29 @@
         <f>Comparatifs!B27</f>
         <v>0</v>
       </c>
-      <c r="C2" s="101" t="s">
+      <c r="C2" s="107" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="101"/>
-      <c r="E2" s="102"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="108"/>
       <c r="G2" s="8">
         <f>Comparatifs!B28+B10</f>
         <v>0</v>
       </c>
-      <c r="H2" s="101" t="s">
+      <c r="H2" s="107" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="101"/>
-      <c r="J2" s="102"/>
+      <c r="I2" s="107"/>
+      <c r="J2" s="108"/>
       <c r="L2" s="8">
         <f>Comparatifs!B29+G9</f>
         <v>0</v>
       </c>
-      <c r="M2" s="101" t="s">
+      <c r="M2" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="N2" s="101"/>
-      <c r="O2" s="102"/>
+      <c r="N2" s="107"/>
+      <c r="O2" s="108"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="10">
@@ -4099,29 +4059,29 @@
         <f>Comparatifs!B12</f>
         <v>0</v>
       </c>
-      <c r="C13" s="101" t="s">
+      <c r="C13" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="101"/>
-      <c r="E13" s="102"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="108"/>
       <c r="G13" s="8">
         <f>Comparatifs!B14+B21</f>
         <v>0</v>
       </c>
-      <c r="H13" s="101" t="s">
+      <c r="H13" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="101"/>
-      <c r="J13" s="102"/>
+      <c r="I13" s="107"/>
+      <c r="J13" s="108"/>
       <c r="L13" s="8">
         <f>Comparatifs!B13+G20</f>
         <v>0</v>
       </c>
-      <c r="M13" s="101" t="s">
+      <c r="M13" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="N13" s="101"/>
-      <c r="O13" s="102"/>
+      <c r="N13" s="107"/>
+      <c r="O13" s="108"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
@@ -4488,29 +4448,29 @@
         <f>Comparatifs!B15</f>
         <v>5</v>
       </c>
-      <c r="C24" s="101" t="s">
+      <c r="C24" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="101"/>
-      <c r="E24" s="102"/>
+      <c r="D24" s="107"/>
+      <c r="E24" s="108"/>
       <c r="G24" s="8">
         <f>Comparatifs!B16+B32</f>
         <v>5</v>
       </c>
-      <c r="H24" s="101" t="s">
+      <c r="H24" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="I24" s="101"/>
-      <c r="J24" s="102"/>
+      <c r="I24" s="107"/>
+      <c r="J24" s="108"/>
       <c r="L24" s="8">
         <f>Comparatifs!B17+G31</f>
         <v>5</v>
       </c>
-      <c r="M24" s="101" t="s">
+      <c r="M24" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="N24" s="101"/>
-      <c r="O24" s="102"/>
+      <c r="N24" s="107"/>
+      <c r="O24" s="108"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="10">
@@ -4877,29 +4837,29 @@
         <f>Comparatifs!B18</f>
         <v>0</v>
       </c>
-      <c r="C35" s="101" t="s">
+      <c r="C35" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="101"/>
-      <c r="E35" s="102"/>
+      <c r="D35" s="107"/>
+      <c r="E35" s="108"/>
       <c r="G35" s="8">
         <f>Comparatifs!B19+B43</f>
         <v>0</v>
       </c>
-      <c r="H35" s="101" t="s">
+      <c r="H35" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="I35" s="101"/>
-      <c r="J35" s="102"/>
+      <c r="I35" s="107"/>
+      <c r="J35" s="108"/>
       <c r="L35" s="8">
         <f>Comparatifs!B20+G42</f>
         <v>0</v>
       </c>
-      <c r="M35" s="101" t="s">
+      <c r="M35" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="N35" s="101"/>
-      <c r="O35" s="102"/>
+      <c r="N35" s="107"/>
+      <c r="O35" s="108"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="10">
@@ -5266,29 +5226,29 @@
         <f>Comparatifs!B21</f>
         <v>0</v>
       </c>
-      <c r="C46" s="101" t="s">
+      <c r="C46" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="101"/>
-      <c r="E46" s="102"/>
+      <c r="D46" s="107"/>
+      <c r="E46" s="108"/>
       <c r="G46" s="8">
         <f>Comparatifs!B22+B54</f>
         <v>0</v>
       </c>
-      <c r="H46" s="101" t="s">
+      <c r="H46" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="I46" s="101"/>
-      <c r="J46" s="102"/>
+      <c r="I46" s="107"/>
+      <c r="J46" s="108"/>
       <c r="L46" s="8">
         <f>Comparatifs!B23+G53</f>
         <v>0</v>
       </c>
-      <c r="M46" s="101" t="s">
+      <c r="M46" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="N46" s="101"/>
-      <c r="O46" s="102"/>
+      <c r="N46" s="107"/>
+      <c r="O46" s="108"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="10">
@@ -5655,29 +5615,29 @@
         <f>Comparatifs!B24</f>
         <v>5</v>
       </c>
-      <c r="C57" s="101" t="s">
+      <c r="C57" s="107" t="s">
         <v>60</v>
       </c>
-      <c r="D57" s="101"/>
-      <c r="E57" s="102"/>
+      <c r="D57" s="107"/>
+      <c r="E57" s="108"/>
       <c r="G57" s="8">
         <f>Comparatifs!B25+B65</f>
         <v>5</v>
       </c>
-      <c r="H57" s="101" t="s">
+      <c r="H57" s="107" t="s">
         <v>59</v>
       </c>
-      <c r="I57" s="101"/>
-      <c r="J57" s="102"/>
+      <c r="I57" s="107"/>
+      <c r="J57" s="108"/>
       <c r="L57" s="8">
         <f>Comparatifs!B26+G64</f>
         <v>5</v>
       </c>
-      <c r="M57" s="101" t="s">
+      <c r="M57" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="N57" s="101"/>
-      <c r="O57" s="102"/>
+      <c r="N57" s="107"/>
+      <c r="O57" s="108"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" s="10">
@@ -6044,29 +6004,29 @@
         <f>Comparatifs!B30</f>
         <v>5</v>
       </c>
-      <c r="C68" s="101" t="s">
+      <c r="C68" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="D68" s="101"/>
-      <c r="E68" s="102"/>
+      <c r="D68" s="107"/>
+      <c r="E68" s="108"/>
       <c r="G68" s="8">
         <f>Comparatifs!B31+B76</f>
         <v>5</v>
       </c>
-      <c r="H68" s="101" t="s">
+      <c r="H68" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="I68" s="101"/>
-      <c r="J68" s="102"/>
+      <c r="I68" s="107"/>
+      <c r="J68" s="108"/>
       <c r="L68" s="8">
         <f>Comparatifs!B32+G75</f>
         <v>5</v>
       </c>
-      <c r="M68" s="101" t="s">
+      <c r="M68" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="N68" s="101"/>
-      <c r="O68" s="102"/>
+      <c r="N68" s="107"/>
+      <c r="O68" s="108"/>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B69" s="10">
@@ -6433,29 +6393,29 @@
         <f>Comparatifs!B33</f>
         <v>5</v>
       </c>
-      <c r="C79" s="101" t="s">
+      <c r="C79" s="107" t="s">
         <v>115</v>
       </c>
-      <c r="D79" s="101"/>
-      <c r="E79" s="102"/>
+      <c r="D79" s="107"/>
+      <c r="E79" s="108"/>
       <c r="G79" s="8">
         <f>Comparatifs!B34+B87</f>
         <v>5</v>
       </c>
-      <c r="H79" s="101" t="s">
+      <c r="H79" s="107" t="s">
         <v>114</v>
       </c>
-      <c r="I79" s="101"/>
-      <c r="J79" s="102"/>
+      <c r="I79" s="107"/>
+      <c r="J79" s="108"/>
       <c r="L79" s="8">
         <f>Comparatifs!B35+G86</f>
         <v>5</v>
       </c>
-      <c r="M79" s="101" t="s">
+      <c r="M79" s="107" t="s">
         <v>116</v>
       </c>
-      <c r="N79" s="101"/>
-      <c r="O79" s="102"/>
+      <c r="N79" s="107"/>
+      <c r="O79" s="108"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B80" s="10">
@@ -6822,29 +6782,29 @@
         <f>Comparatifs!B36</f>
         <v>0</v>
       </c>
-      <c r="C90" s="101" t="s">
+      <c r="C90" s="107" t="s">
         <v>124</v>
       </c>
-      <c r="D90" s="101"/>
-      <c r="E90" s="102"/>
+      <c r="D90" s="107"/>
+      <c r="E90" s="108"/>
       <c r="G90" s="8">
         <f>Comparatifs!B37+B98</f>
         <v>0</v>
       </c>
-      <c r="H90" s="101" t="s">
+      <c r="H90" s="107" t="s">
         <v>123</v>
       </c>
-      <c r="I90" s="101"/>
-      <c r="J90" s="102"/>
+      <c r="I90" s="107"/>
+      <c r="J90" s="108"/>
       <c r="L90" s="8">
         <f>Comparatifs!B38+G97</f>
         <v>0</v>
       </c>
-      <c r="M90" s="101" t="s">
+      <c r="M90" s="107" t="s">
         <v>125</v>
       </c>
-      <c r="N90" s="101"/>
-      <c r="O90" s="102"/>
+      <c r="N90" s="107"/>
+      <c r="O90" s="108"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B91" s="10">
@@ -7207,17 +7167,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="H79:J79"/>
-    <mergeCell ref="M79:O79"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="M46:O46"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="H68:J68"/>
-    <mergeCell ref="M68:O68"/>
     <mergeCell ref="C90:E90"/>
     <mergeCell ref="H90:J90"/>
     <mergeCell ref="M90:O90"/>
@@ -7234,6 +7183,17 @@
     <mergeCell ref="H24:J24"/>
     <mergeCell ref="M24:O24"/>
     <mergeCell ref="C35:E35"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="H79:J79"/>
+    <mergeCell ref="M79:O79"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="M46:O46"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="H68:J68"/>
+    <mergeCell ref="M68:O68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7307,16 +7267,16 @@
       <c r="D7" s="40"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="104"/>
-      <c r="G8" s="104"/>
-      <c r="H8" s="104"/>
-      <c r="I8" s="105"/>
+      <c r="C8" s="110"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="110"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="111"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="39"/>
@@ -8290,28 +8250,28 @@
     <mergeCell ref="B8:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="G10 G12:G1048576">
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10 H12:H1048576">
-    <cfRule type="cellIs" dxfId="33" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="greaterThan">
       <formula>40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10 G12:G1048576">
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="greaterThan">
       <formula>500000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G7 G9:G1048576">
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="between">
       <formula>300000</formula>
       <formula>499999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H7 H9:H1048576">
-    <cfRule type="cellIs" dxfId="30" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="between">
       <formula>20</formula>
       <formula>39.99</formula>
     </cfRule>
@@ -8503,7 +8463,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8539,25 +8499,25 @@
         <f>'Comparatifs Idoles'!B12</f>
         <v>1</v>
       </c>
-      <c r="C2" s="101" t="s">
+      <c r="C2" s="107" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="101"/>
-      <c r="E2" s="102"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="108"/>
       <c r="G2" s="8">
         <f>'Comparatifs Idoles'!B13</f>
         <v>0</v>
       </c>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="102"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="107"/>
+      <c r="J2" s="108"/>
       <c r="L2" s="8">
         <f>Comparatifs!B13+G9</f>
         <v>0</v>
       </c>
-      <c r="M2" s="101"/>
-      <c r="N2" s="101"/>
-      <c r="O2" s="102"/>
+      <c r="M2" s="107"/>
+      <c r="N2" s="107"/>
+      <c r="O2" s="108"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="10">
@@ -8881,16 +8841,16 @@
       <c r="D7" s="40"/>
     </row>
     <row r="8" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="109" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="104"/>
-      <c r="G8" s="104"/>
-      <c r="H8" s="104"/>
-      <c r="I8" s="105"/>
+      <c r="C8" s="110"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="110"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="111"/>
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="39"/>
@@ -8987,40 +8947,40 @@
     <mergeCell ref="B8:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="G10 G12:G1048576">
-    <cfRule type="cellIs" dxfId="28" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10 H12:H1048576">
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="greaterThan">
       <formula>40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10 G12:G1048576">
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="greaterThan">
       <formula>500000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G6 G10:G1048576">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="between">
       <formula>300000</formula>
       <formula>499999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H6 H10:H1048576">
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="between">
       <formula>20</formula>
       <formula>39.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7 G9">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="between">
       <formula>300000</formula>
       <formula>499999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7 H9">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="between">
       <formula>20</formula>
       <formula>39.99</formula>
     </cfRule>
@@ -9107,11 +9067,11 @@
       <c r="B9" s="8">
         <v>0</v>
       </c>
-      <c r="C9" s="101" t="s">
+      <c r="C9" s="107" t="s">
         <v>91</v>
       </c>
-      <c r="D9" s="101"/>
-      <c r="E9" s="106"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="112"/>
       <c r="F9" s="48"/>
       <c r="H9" t="s">
         <v>8</v>
@@ -9316,11 +9276,11 @@
         <f>G11</f>
         <v>1</v>
       </c>
-      <c r="C20" s="101" t="s">
+      <c r="C20" s="107" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="101"/>
-      <c r="E20" s="106"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="112"/>
       <c r="F20" s="48"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -9661,19 +9621,19 @@
     <mergeCell ref="C20:E20"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G7">
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="between">
       <formula>300000</formula>
       <formula>499999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H7">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="between">
       <formula>20</formula>
       <formula>39.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:C45">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9687,7 +9647,7 @@
   <dimension ref="B1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9772,7 +9732,7 @@
         <f t="shared" ref="I4:I12" si="0">C18</f>
         <v>36994</v>
       </c>
-      <c r="J4" s="107" t="str">
+      <c r="J4" s="101" t="str">
         <f>C32</f>
         <v>119996</v>
       </c>
@@ -9780,11 +9740,11 @@
         <f>I4-G4-(I4*0.01)</f>
         <v>-14369.94</v>
       </c>
-      <c r="L4" s="109">
+      <c r="L4" s="103">
         <f t="shared" ref="L4:L14" si="1">1-(G4/I4)</f>
         <v>-0.37843974698599769</v>
       </c>
-      <c r="M4" s="111">
+      <c r="M4" s="105">
         <f>K4/G4</f>
         <v>-0.28179668196258384</v>
       </c>
@@ -9792,7 +9752,7 @@
         <f>J4-H4-(J4*0.01)</f>
         <v>-34185.96</v>
       </c>
-      <c r="O4" s="109">
+      <c r="O4" s="103">
         <f>N4/H4</f>
         <v>-0.22346393693375691</v>
       </c>
@@ -9828,7 +9788,7 @@
         <f t="shared" si="0"/>
         <v>31995</v>
       </c>
-      <c r="J5" s="108">
+      <c r="J5" s="102">
         <f t="shared" ref="J5:J11" si="3">C33</f>
         <v>100000</v>
       </c>
@@ -9836,11 +9796,11 @@
         <f t="shared" ref="K5:K16" si="4">I5-G5-(I5*0.01)</f>
         <v>2617.0500000000002</v>
       </c>
-      <c r="L5" s="110">
+      <c r="L5" s="104">
         <f t="shared" si="1"/>
         <v>9.1795593061415826E-2</v>
       </c>
-      <c r="M5" s="112">
+      <c r="M5" s="106">
         <f t="shared" ref="M5:M7" si="5">K5/G5</f>
         <v>9.0062977493289287E-2</v>
       </c>
@@ -9848,7 +9808,7 @@
         <f t="shared" ref="N5:N11" si="6">J5-H5-(J5*0.01)</f>
         <v>11826</v>
       </c>
-      <c r="O5" s="109">
+      <c r="O5" s="103">
         <f t="shared" ref="O5:O11" si="7">N5/H5</f>
         <v>0.13565971505265331</v>
       </c>
@@ -9884,7 +9844,7 @@
         <f t="shared" si="0"/>
         <v>12579</v>
       </c>
-      <c r="J6" s="108" t="str">
+      <c r="J6" s="102" t="str">
         <f t="shared" si="3"/>
         <v>37365</v>
       </c>
@@ -9892,11 +9852,11 @@
         <f t="shared" si="4"/>
         <v>516.21</v>
       </c>
-      <c r="L6" s="110">
+      <c r="L6" s="104">
         <f t="shared" si="1"/>
         <v>5.1037443357977552E-2</v>
       </c>
-      <c r="M6" s="112">
+      <c r="M6" s="106">
         <f t="shared" si="5"/>
         <v>4.3244533802462931E-2</v>
       </c>
@@ -9904,7 +9864,7 @@
         <f t="shared" si="6"/>
         <v>1180.3499999999999</v>
       </c>
-      <c r="O6" s="109">
+      <c r="O6" s="103">
         <f t="shared" si="7"/>
         <v>3.2960542849962297E-2</v>
       </c>
@@ -9940,7 +9900,7 @@
         <f t="shared" si="0"/>
         <v>24997</v>
       </c>
-      <c r="J7" s="108" t="str">
+      <c r="J7" s="102" t="str">
         <f t="shared" si="3"/>
         <v>76499</v>
       </c>
@@ -9948,11 +9908,11 @@
         <f t="shared" si="4"/>
         <v>2148.0300000000002</v>
       </c>
-      <c r="L7" s="110">
+      <c r="L7" s="104">
         <f t="shared" si="1"/>
         <v>9.5931511781413792E-2</v>
       </c>
-      <c r="M7" s="112">
+      <c r="M7" s="106">
         <f t="shared" si="5"/>
         <v>9.5049780963759462E-2</v>
       </c>
@@ -9960,7 +9920,7 @@
         <f t="shared" si="6"/>
         <v>7937.01</v>
       </c>
-      <c r="O7" s="109">
+      <c r="O7" s="103">
         <f t="shared" si="7"/>
         <v>0.11707022434621001</v>
       </c>
@@ -9996,7 +9956,7 @@
         <f t="shared" si="0"/>
         <v>56400</v>
       </c>
-      <c r="J8" s="108" t="str">
+      <c r="J8" s="102" t="str">
         <f t="shared" si="3"/>
         <v>147800</v>
       </c>
@@ -10004,11 +9964,11 @@
         <f t="shared" si="4"/>
         <v>9363</v>
       </c>
-      <c r="L8" s="110">
+      <c r="L8" s="104">
         <f t="shared" si="1"/>
         <v>0.17601063829787233</v>
       </c>
-      <c r="M8" s="112">
+      <c r="M8" s="106">
         <f>K8/G8</f>
         <v>0.20147182234846039</v>
       </c>
@@ -10016,7 +9976,7 @@
         <f t="shared" si="6"/>
         <v>6903</v>
       </c>
-      <c r="O8" s="109">
+      <c r="O8" s="103">
         <f t="shared" si="7"/>
         <v>4.951262023110193E-2</v>
       </c>
@@ -10052,7 +10012,7 @@
         <f t="shared" si="0"/>
         <v>58986</v>
       </c>
-      <c r="J9" s="108" t="str">
+      <c r="J9" s="102" t="str">
         <f t="shared" si="3"/>
         <v>168997</v>
       </c>
@@ -10060,11 +10020,11 @@
         <f t="shared" si="4"/>
         <v>-1180.8600000000001</v>
       </c>
-      <c r="L9" s="110">
+      <c r="L9" s="104">
         <f t="shared" si="1"/>
         <v>-1.0019326619875812E-2</v>
       </c>
-      <c r="M9" s="112">
+      <c r="M9" s="106">
         <f>K9/G9</f>
         <v>-1.9820736190140492E-2</v>
       </c>
@@ -10072,7 +10032,7 @@
         <f t="shared" si="6"/>
         <v>-11423.97</v>
       </c>
-      <c r="O9" s="109">
+      <c r="O9" s="103">
         <f t="shared" si="7"/>
         <v>-6.3917115665441351E-2</v>
       </c>
@@ -10108,7 +10068,7 @@
         <f t="shared" si="0"/>
         <v>38997</v>
       </c>
-      <c r="J10" s="108" t="str">
+      <c r="J10" s="102" t="str">
         <f t="shared" si="3"/>
         <v>98948</v>
       </c>
@@ -10116,11 +10076,11 @@
         <f t="shared" si="4"/>
         <v>-1574.97</v>
       </c>
-      <c r="L10" s="110">
+      <c r="L10" s="104">
         <f t="shared" si="1"/>
         <v>-3.0386952842526238E-2</v>
       </c>
-      <c r="M10" s="112">
+      <c r="M10" s="106">
         <f t="shared" ref="M10:M16" si="10">K10/G10</f>
         <v>-3.9195908615798122E-2</v>
       </c>
@@ -10128,7 +10088,7 @@
         <f t="shared" si="6"/>
         <v>-22587.48</v>
       </c>
-      <c r="O10" s="109">
+      <c r="O10" s="103">
         <f t="shared" si="7"/>
         <v>-0.18737643721069136</v>
       </c>
@@ -10141,55 +10101,56 @@
       <c r="B11" s="95" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="3">
-        <v>54989</v>
+      <c r="C11" s="3" t="str">
+        <f>Raw!D16</f>
+        <v>27890</v>
       </c>
       <c r="E11" s="76" t="s">
         <v>171</v>
       </c>
-      <c r="F11" s="73">
+      <c r="F11" s="73" t="str">
         <f t="shared" si="9"/>
-        <v>54989</v>
+        <v>27890</v>
       </c>
       <c r="G11" s="74">
         <f t="shared" si="2"/>
-        <v>164967</v>
+        <v>83670</v>
       </c>
       <c r="H11" s="74">
         <f t="shared" si="2"/>
-        <v>494901</v>
+        <v>251010</v>
       </c>
       <c r="I11" s="91" t="str">
         <f t="shared" si="0"/>
         <v>92882</v>
       </c>
-      <c r="J11" s="108">
+      <c r="J11" s="102">
         <f t="shared" si="3"/>
-        <v>519750</v>
+        <v>220000</v>
       </c>
       <c r="K11" s="21">
         <f t="shared" si="4"/>
-        <v>-73013.820000000007</v>
-      </c>
-      <c r="L11" s="110">
+        <v>8283.18</v>
+      </c>
+      <c r="L11" s="104">
         <f t="shared" si="1"/>
-        <v>-0.77609224607566585</v>
-      </c>
-      <c r="M11" s="112">
+        <v>9.9179604229021723E-2</v>
+      </c>
+      <c r="M11" s="106">
         <f t="shared" si="10"/>
-        <v>-0.44259651930386079</v>
+        <v>9.8998207242739333E-2</v>
       </c>
       <c r="N11" s="22">
         <f t="shared" si="6"/>
-        <v>19651.5</v>
-      </c>
-      <c r="O11" s="109">
+        <v>-33210</v>
+      </c>
+      <c r="O11" s="103">
         <f t="shared" si="7"/>
-        <v>3.9707941588317662E-2</v>
+        <v>-0.13230548583721763</v>
       </c>
       <c r="P11" s="70">
         <f t="shared" si="8"/>
-        <v>4.7809523809523857E-2</v>
+        <v>-0.14095454545454555</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
@@ -10211,20 +10172,17 @@
         <f t="shared" si="2"/>
         <v>112776</v>
       </c>
-      <c r="H12" s="74">
-        <f t="shared" si="2"/>
-        <v>338328</v>
-      </c>
+      <c r="H12" s="74"/>
       <c r="I12" s="91" t="str">
         <f t="shared" si="0"/>
         <v>129600</v>
       </c>
-      <c r="J12" s="108"/>
+      <c r="J12" s="102"/>
       <c r="K12" s="21">
         <f t="shared" si="4"/>
         <v>15528</v>
       </c>
-      <c r="L12" s="110">
+      <c r="L12" s="104">
         <f t="shared" si="1"/>
         <v>0.12981481481481483</v>
       </c>
@@ -10255,20 +10213,17 @@
         <f t="shared" si="2"/>
         <v>301797</v>
       </c>
-      <c r="H13" s="74">
-        <f t="shared" si="2"/>
-        <v>905391</v>
-      </c>
+      <c r="H13" s="74"/>
       <c r="I13" s="91" t="str">
         <f t="shared" ref="I13:I16" si="11">C27</f>
         <v>335800</v>
       </c>
-      <c r="J13" s="108"/>
+      <c r="J13" s="102"/>
       <c r="K13" s="21">
         <f t="shared" si="4"/>
         <v>30645</v>
       </c>
-      <c r="L13" s="110">
+      <c r="L13" s="104">
         <f t="shared" si="1"/>
         <v>0.10125967837998806</v>
       </c>
@@ -10299,20 +10254,17 @@
         <f t="shared" si="2"/>
         <v>326400</v>
       </c>
-      <c r="H14" s="74">
-        <f t="shared" si="2"/>
-        <v>979200</v>
-      </c>
+      <c r="H14" s="74"/>
       <c r="I14" s="91" t="str">
         <f t="shared" si="11"/>
         <v>389886</v>
       </c>
-      <c r="J14" s="108"/>
+      <c r="J14" s="102"/>
       <c r="K14" s="21">
         <f t="shared" si="4"/>
         <v>59587.14</v>
       </c>
-      <c r="L14" s="110">
+      <c r="L14" s="104">
         <f t="shared" si="1"/>
         <v>0.16283221249288249</v>
       </c>
@@ -10343,20 +10295,17 @@
         <f t="shared" si="2"/>
         <v>276888</v>
       </c>
-      <c r="H15" s="74">
-        <f t="shared" si="2"/>
-        <v>830664</v>
-      </c>
+      <c r="H15" s="74"/>
       <c r="I15" s="91" t="str">
         <f t="shared" si="11"/>
         <v>319792</v>
       </c>
-      <c r="J15" s="108"/>
+      <c r="J15" s="102"/>
       <c r="K15" s="21">
         <f t="shared" si="4"/>
         <v>39706.080000000002</v>
       </c>
-      <c r="L15" s="110">
+      <c r="L15" s="104">
         <f>1-(G15/I15)</f>
         <v>0.13416220543353174</v>
       </c>
@@ -10387,20 +10336,17 @@
         <f t="shared" si="2"/>
         <v>206991</v>
       </c>
-      <c r="H16" s="74">
-        <f t="shared" si="2"/>
-        <v>620973</v>
-      </c>
+      <c r="H16" s="74"/>
       <c r="I16" s="91" t="str">
         <f t="shared" si="11"/>
         <v>228995</v>
       </c>
-      <c r="J16" s="108"/>
+      <c r="J16" s="102"/>
       <c r="K16" s="22">
         <f t="shared" si="4"/>
         <v>19714.05</v>
       </c>
-      <c r="L16" s="110">
+      <c r="L16" s="104">
         <f>1-(G16/I16)</f>
         <v>9.6089434267123686E-2</v>
       </c>
@@ -10603,66 +10549,67 @@
         <v>163</v>
       </c>
       <c r="C39" s="22">
-        <v>519750</v>
+        <f>Raw!D68</f>
+        <v>220000</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K4:K16">
-    <cfRule type="cellIs" dxfId="5" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="greaterThan">
       <formula>5000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12:O12 N4:N11">
-    <cfRule type="cellIs" dxfId="18" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="greaterThan">
       <formula>5000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P12">
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="lessThan">
       <formula>0.0001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="greaterThan">
       <formula>0.25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="between">
       <formula>0.15</formula>
       <formula>0.25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="greaterThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:M16">
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="lessThan">
       <formula>0.0001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="greaterThan">
       <formula>0.25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="between">
       <formula>0.15</formula>
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G16">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
       <formula>$F$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:O11">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0.0001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0.25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
       <formula>0.15</formula>
       <formula>0.25</formula>
     </cfRule>
@@ -10676,7 +10623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>

</xml_diff>